<commit_message>
Add data validation to groepen en niet_samen
</commit_message>
<xml_diff>
--- a/input_templates/groepen.xlsx
+++ b/input_templates/groepen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjoer\Documents\Willekeurige berekeningen\leerlingindeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjoer\Documents\Willekeurige berekeningen\aliexpress\input_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F9639-FDF4-42B4-8BC7-8900A6F831A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E486704A-767B-4FAC-AF04-A539052E02CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{936DD519-497D-4C4F-8EC6-21D9C0CBD05E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{936DD519-497D-4C4F-8EC6-21D9C0CBD05E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,8 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,22 +422,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F1FFEC-EE39-461A-A28C-ABC789923C21}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="oxpEbE+eD3ttAikPf3wXYCerw0cWucHJAmjATC6l1u9vYf0gevy5zicZTS0FIJWjpDf5Aebizd30DomZF5/UNQ==" saltValue="ceTnBYUrXw+QWM1HmmxaGA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Vul een geheel getal in" sqref="B2:C1048576" xr:uid="{6C0A9AFA-B9D7-428B-8AC2-AEF8C495C45B}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Groepen" prompt="De naam van de groep waar leerlingen naar toe gaan" sqref="A1" xr:uid="{0D0A292D-52F8-4297-A423-DE5FBA94D85E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Aantal jongens" prompt="Het aantal jongens in de groep wat overblijft nadat de oude leerlingen zijn vertrokken." sqref="B1" xr:uid="{DEDA2B8E-B8A6-4504-8A90-30B884AC0A4A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Aantal meisjes" prompt="Het aantal meisjes in de groep wat overblijft nadat de oude leerlingen zijn vertrokken." sqref="C1" xr:uid="{C3763C86-4E32-43D6-B7D2-C37487BBD0D5}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>